<commit_message>
Added MPI SVD results
</commit_message>
<xml_diff>
--- a/Virtualization/singularity.xlsx
+++ b/Virtualization/singularity.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="888" yWindow="0" windowWidth="13608" windowHeight="5736"/>
+    <workbookView xWindow="1776" yWindow="0" windowWidth="13608" windowHeight="5736" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="OpenMP" sheetId="1" r:id="rId1"/>
+    <sheet name="MPI" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
   <si>
     <t>cores</t>
   </si>
@@ -54,6 +55,45 @@
   </si>
   <si>
     <t>weak scaling results</t>
+  </si>
+  <si>
+    <t>nodes</t>
+  </si>
+  <si>
+    <t>cores/node</t>
+  </si>
+  <si>
+    <t>processes</t>
+  </si>
+  <si>
+    <t>matrix dim.</t>
+  </si>
+  <si>
+    <t>singularity DGEMM (s)</t>
+  </si>
+  <si>
+    <t>singularity SVD (s)</t>
+  </si>
+  <si>
+    <t>native HDF5 (s)</t>
+  </si>
+  <si>
+    <t>native SVD (s)</t>
+  </si>
+  <si>
+    <t>native DGEMM (s)</t>
+  </si>
+  <si>
+    <t>singularity HDF5 (s)</t>
+  </si>
+  <si>
+    <t>HDF5 overhead</t>
+  </si>
+  <si>
+    <t>SVD overhead</t>
+  </si>
+  <si>
+    <t>DGEMM overhead</t>
   </si>
 </sst>
 </file>
@@ -179,7 +219,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -197,6 +237,7 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
@@ -480,7 +521,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
@@ -981,4 +1022,121 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:M2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <f>A2*B2</f>
+        <v>16</v>
+      </c>
+      <c r="D2">
+        <v>5000</v>
+      </c>
+      <c r="E2" s="15">
+        <v>1.8913409999999999</v>
+      </c>
+      <c r="F2" s="15">
+        <v>68.060210999999995</v>
+      </c>
+      <c r="G2" s="15">
+        <v>2.5266380000000002</v>
+      </c>
+      <c r="H2" s="15">
+        <v>2.4477449999999998</v>
+      </c>
+      <c r="I2" s="15">
+        <v>99.785908000000006</v>
+      </c>
+      <c r="J2" s="15">
+        <v>12.625704000000001</v>
+      </c>
+      <c r="K2" s="15">
+        <f>H2/E2</f>
+        <v>1.2941849195887996</v>
+      </c>
+      <c r="L2" s="15">
+        <f>I2/F2</f>
+        <v>1.4661416198077908</v>
+      </c>
+      <c r="M2" s="15">
+        <f>J2/G2</f>
+        <v>4.9970371695510005</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added MPI 1 process results
</commit_message>
<xml_diff>
--- a/Virtualization/singularity.xlsx
+++ b/Virtualization/singularity.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1776" yWindow="0" windowWidth="13608" windowHeight="5736" activeTab="1"/>
+    <workbookView xWindow="2664" yWindow="0" windowWidth="13608" windowHeight="5736" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="OpenMP" sheetId="1" r:id="rId1"/>
@@ -1026,10 +1026,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:M2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1135,6 +1135,51 @@
         <v>4.9970371695510005</v>
       </c>
     </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <f>A3*B3</f>
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>5000</v>
+      </c>
+      <c r="E3" s="15">
+        <v>2.245485</v>
+      </c>
+      <c r="F3" s="15">
+        <v>790.76326800000004</v>
+      </c>
+      <c r="G3" s="15">
+        <v>19.051117000000001</v>
+      </c>
+      <c r="H3" s="15">
+        <v>2.3856459999999999</v>
+      </c>
+      <c r="I3" s="15">
+        <v>1166.8051579999999</v>
+      </c>
+      <c r="J3" s="15">
+        <v>233.70181199999999</v>
+      </c>
+      <c r="K3" s="15">
+        <f>H3/E3</f>
+        <v>1.0624190319685947</v>
+      </c>
+      <c r="L3" s="15">
+        <f>I3/F3</f>
+        <v>1.4755429408741831</v>
+      </c>
+      <c r="M3" s="15">
+        <f>J3/G3</f>
+        <v>12.267092370489351</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added more MPI results; added serial results for SVD; imporved formatting
</commit_message>
<xml_diff>
--- a/Virtualization/singularity.xlsx
+++ b/Virtualization/singularity.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2664" yWindow="0" windowWidth="13608" windowHeight="5736" activeTab="1"/>
+    <workbookView xWindow="4440" yWindow="0" windowWidth="13608" windowHeight="5736" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="OpenMP" sheetId="1" r:id="rId1"/>
     <sheet name="MPI" sheetId="2" r:id="rId2"/>
+    <sheet name="serial" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="24">
   <si>
     <t>cores</t>
   </si>
@@ -94,6 +95,30 @@
   </si>
   <si>
     <t>DGEMM overhead</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">computing </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>p</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -104,7 +129,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -127,8 +152,39 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Symbol"/>
+      <family val="1"/>
+      <charset val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -138,6 +194,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -215,11 +277,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -237,10 +300,17 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="2" builtinId="32"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -519,10 +589,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -535,7 +605,7 @@
     <col min="6" max="6" width="24.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -555,7 +625,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -578,7 +648,7 @@
         <v>6.8041675526259891E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -601,7 +671,7 @@
         <v>9.5561690380123031E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>4</v>
       </c>
@@ -626,8 +696,11 @@
       <c r="H4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K4" s="15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>8</v>
       </c>
@@ -650,7 +723,7 @@
         <v>1.8644067796610188E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>16</v>
       </c>
@@ -673,7 +746,7 @@
         <v>3.0431107354184302E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>28</v>
       </c>
@@ -696,7 +769,7 @@
         <v>4.6715328467153164E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>0</v>
       </c>
@@ -716,7 +789,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>1</v>
       </c>
@@ -739,7 +812,7 @@
         <v>6.5366423978318071E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>2</v>
       </c>
@@ -762,7 +835,7 @@
         <v>7.5906364456712503E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>4</v>
       </c>
@@ -788,7 +861,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>8</v>
       </c>
@@ -811,7 +884,7 @@
         <v>7.4215436810856957E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>16</v>
       </c>
@@ -834,7 +907,7 @@
         <v>8.1632653061224445E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="6">
         <v>28</v>
       </c>
@@ -1026,158 +1099,298 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="20" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="A2" s="2">
+        <v>8</v>
+      </c>
+      <c r="B2" s="4">
+        <v>8</v>
+      </c>
+      <c r="C2" s="4">
+        <f>A2*B2</f>
+        <v>64</v>
+      </c>
+      <c r="D2" s="4">
+        <v>5000</v>
+      </c>
+      <c r="E2" s="16">
+        <v>6.5709160000000004</v>
+      </c>
+      <c r="F2" s="16">
+        <v>21.975985999999999</v>
+      </c>
+      <c r="G2" s="16">
+        <v>0.66231899999999999</v>
+      </c>
+      <c r="H2" s="16">
+        <v>6.7748900000000001</v>
+      </c>
+      <c r="I2" s="16">
+        <v>27.178031000000001</v>
+      </c>
+      <c r="J2" s="16">
+        <v>0.72076600000000002</v>
+      </c>
+      <c r="K2" s="16">
+        <f t="shared" ref="K2" si="0">H2/E2</f>
+        <v>1.0310419430106852</v>
+      </c>
+      <c r="L2" s="16">
+        <f t="shared" ref="L2" si="1">I2/F2</f>
+        <v>1.2367149760652378</v>
+      </c>
+      <c r="M2" s="17">
+        <f t="shared" ref="M2" si="2">J2/G2</f>
+        <v>1.0882459962646398</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B2">
+      <c r="B3" s="4">
         <v>8</v>
       </c>
-      <c r="C2">
-        <f>A2*B2</f>
+      <c r="C3" s="4">
+        <f>A3*B3</f>
         <v>16</v>
       </c>
-      <c r="D2">
+      <c r="D3" s="4">
         <v>5000</v>
       </c>
-      <c r="E2" s="15">
+      <c r="E3" s="16">
         <v>1.8913409999999999</v>
       </c>
-      <c r="F2" s="15">
+      <c r="F3" s="16">
         <v>68.060210999999995</v>
       </c>
-      <c r="G2" s="15">
+      <c r="G3" s="16">
         <v>2.5266380000000002</v>
       </c>
-      <c r="H2" s="15">
-        <v>2.4477449999999998</v>
-      </c>
-      <c r="I2" s="15">
-        <v>99.785908000000006</v>
-      </c>
-      <c r="J2" s="15">
-        <v>12.625704000000001</v>
-      </c>
-      <c r="K2" s="15">
-        <f>H2/E2</f>
-        <v>1.2941849195887996</v>
-      </c>
-      <c r="L2" s="15">
-        <f>I2/F2</f>
-        <v>1.4661416198077908</v>
-      </c>
-      <c r="M2" s="15">
-        <f>J2/G2</f>
-        <v>4.9970371695510005</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="H3" s="16">
+        <v>2.2257220000000002</v>
+      </c>
+      <c r="I3" s="16">
+        <v>73.004705999999999</v>
+      </c>
+      <c r="J3" s="16">
+        <v>2.4950130000000001</v>
+      </c>
+      <c r="K3" s="16">
+        <f t="shared" ref="K3:M4" si="3">H3/E3</f>
+        <v>1.176795723246099</v>
+      </c>
+      <c r="L3" s="16">
+        <f t="shared" si="3"/>
+        <v>1.0726488344269165</v>
+      </c>
+      <c r="M3" s="17">
+        <f t="shared" si="3"/>
+        <v>0.98748336722553842</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="6">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="B4" s="8">
         <v>1</v>
       </c>
-      <c r="C3">
-        <f>A3*B3</f>
+      <c r="C4" s="8">
+        <f>A4*B4</f>
         <v>1</v>
       </c>
-      <c r="D3">
+      <c r="D4" s="8">
         <v>5000</v>
       </c>
-      <c r="E3" s="15">
+      <c r="E4" s="18">
         <v>2.245485</v>
       </c>
-      <c r="F3" s="15">
+      <c r="F4" s="18">
         <v>790.76326800000004</v>
       </c>
-      <c r="G3" s="15">
+      <c r="G4" s="18">
         <v>19.051117000000001</v>
       </c>
-      <c r="H3" s="15">
+      <c r="H4" s="18">
         <v>2.3856459999999999</v>
       </c>
-      <c r="I3" s="15">
-        <v>1166.8051579999999</v>
-      </c>
-      <c r="J3" s="15">
-        <v>233.70181199999999</v>
-      </c>
-      <c r="K3" s="15">
-        <f>H3/E3</f>
+      <c r="I4" s="18">
+        <v>836.88677499999994</v>
+      </c>
+      <c r="J4" s="18">
+        <v>19.256658999999999</v>
+      </c>
+      <c r="K4" s="18">
+        <f t="shared" si="3"/>
         <v>1.0624190319685947</v>
       </c>
-      <c r="L3" s="15">
-        <f>I3/F3</f>
-        <v>1.4755429408741831</v>
-      </c>
-      <c r="M3" s="15">
-        <f>J3/G3</f>
-        <v>12.267092370489351</v>
+      <c r="L4" s="18">
+        <f t="shared" si="3"/>
+        <v>1.05832783193971</v>
+      </c>
+      <c r="M4" s="19">
+        <f t="shared" si="3"/>
+        <v>1.0107889736858997</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" s="21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="6">
+        <v>5000</v>
+      </c>
+      <c r="B2" s="7">
+        <v>1.8513703610000001</v>
+      </c>
+      <c r="C2" s="7">
+        <v>637.64700000000005</v>
+      </c>
+      <c r="D2" s="7">
+        <v>19.334800000000001</v>
+      </c>
+      <c r="E2" s="7">
+        <v>2.8504550000000002</v>
+      </c>
+      <c r="F2" s="7">
+        <v>698.07074999999998</v>
+      </c>
+      <c r="G2" s="7">
+        <v>19.324884699999998</v>
+      </c>
+      <c r="H2" s="7">
+        <f>E2/B2</f>
+        <v>1.5396460157547052</v>
+      </c>
+      <c r="I2" s="7">
+        <f>F2/C2</f>
+        <v>1.0947605022841791</v>
+      </c>
+      <c r="J2" s="9">
+        <f>G2/D2</f>
+        <v>0.99948717855886782</v>
       </c>
     </row>
   </sheetData>

</xml_diff>